<commit_message>
CS0504: Actualización de esqueleto de guion
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion04/EsqueletoGuion_CS_05_04_CO.xlsx
+++ b/fuentes/contenidos/grado05/guion04/EsqueletoGuion_CS_05_04_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="83">
   <si>
     <t>FICHA</t>
   </si>
@@ -1752,7 +1752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1913,7 +1913,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,7 +1993,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>60</v>
@@ -2504,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="C81" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3180,6 +3180,9 @@
       <c r="B38" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F38" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G38" s="3" t="s">
         <v>48</v>
       </c>
@@ -3191,6 +3194,9 @@
       <c r="B39" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F39" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G39" s="3" t="s">
         <v>47</v>
       </c>
@@ -3202,6 +3208,9 @@
       <c r="B40" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F40" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="G40" s="3" t="s">
         <v>52</v>
       </c>
@@ -3233,6 +3242,9 @@
       <c r="B42" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F42" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="G42" s="3" t="s">
         <v>48</v>
       </c>
@@ -3244,6 +3256,9 @@
       <c r="B43" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F43" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="G43" s="3" t="s">
         <v>47</v>
       </c>
@@ -3269,6 +3284,9 @@
       <c r="B45" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F45" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="G45" s="3" t="s">
         <v>48</v>
       </c>
@@ -3280,6 +3298,9 @@
       <c r="B46" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F46" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="G46" s="3" t="s">
         <v>47</v>
       </c>
@@ -3291,6 +3312,9 @@
       <c r="B47" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F47" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="G47" s="3" t="s">
         <v>52</v>
       </c>
@@ -3308,6 +3332,9 @@
       <c r="B48" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="F48" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="G48" s="3" t="s">
         <v>51</v>
       </c>
@@ -3326,35 +3353,44 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D50" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="E50" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D51" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="E51" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D52" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="F52" s="18" t="s">
         <v>65</v>
       </c>
@@ -3362,35 +3398,50 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D53" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G53" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D54" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G54" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D55" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="F55" s="18" t="s">
         <v>66</v>
       </c>
@@ -3398,35 +3449,50 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D56" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="G56" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D57" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="G57" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D58" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="F58" s="18" t="s">
         <v>67</v>
       </c>
@@ -3434,46 +3500,70 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D59" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="G59" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D60" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="G60" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D61" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="G61" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D62" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="G62" s="3" t="s">
         <v>52</v>
       </c>
@@ -3484,13 +3574,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D63" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="G63" s="3" t="s">
         <v>68</v>
       </c>
@@ -3550,6 +3646,9 @@
       <c r="B67" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D67" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="E67" s="3" t="s">
         <v>48</v>
       </c>
@@ -3561,6 +3660,9 @@
       <c r="B68" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D68" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="E68" s="3" t="s">
         <v>47</v>
       </c>
@@ -3586,6 +3688,9 @@
       <c r="B70" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D70" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="E70" s="3" t="s">
         <v>48</v>
       </c>
@@ -3597,6 +3702,9 @@
       <c r="B71" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D71" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="E71" s="3" t="s">
         <v>47</v>
       </c>
@@ -3622,6 +3730,9 @@
       <c r="B73" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D73" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="E73" s="3" t="s">
         <v>48</v>
       </c>
@@ -3633,6 +3744,9 @@
       <c r="B74" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D74" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="E74" s="3" t="s">
         <v>47</v>
       </c>
@@ -3644,6 +3758,9 @@
       <c r="B75" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D75" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="E75" s="3" t="s">
         <v>51</v>
       </c>
@@ -3655,6 +3772,9 @@
       <c r="B76" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D76" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="E76" s="3" t="s">
         <v>52</v>
       </c>
@@ -3672,6 +3792,9 @@
       <c r="B77" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D77" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="E77" s="3" t="s">
         <v>68</v>
       </c>
@@ -3767,6 +3890,9 @@
       <c r="B84" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D84" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="E84" s="3" t="s">
         <v>48</v>
       </c>
@@ -3778,6 +3904,9 @@
       <c r="B85" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D85" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="E85" s="3" t="s">
         <v>47</v>
       </c>
@@ -3803,6 +3932,9 @@
       <c r="B87" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D87" s="18" t="s">
+        <v>74</v>
+      </c>
       <c r="E87" s="3" t="s">
         <v>48</v>
       </c>
@@ -3814,6 +3946,9 @@
       <c r="B88" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D88" s="18" t="s">
+        <v>74</v>
+      </c>
       <c r="E88" s="3" t="s">
         <v>47</v>
       </c>
@@ -3839,6 +3974,9 @@
       <c r="B90" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D90" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="E90" s="3" t="s">
         <v>48</v>
       </c>
@@ -3850,6 +3988,9 @@
       <c r="B91" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D91" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="E91" s="3" t="s">
         <v>47</v>
       </c>
@@ -3861,6 +4002,9 @@
       <c r="B92" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D92" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="E92" s="3" t="s">
         <v>51</v>
       </c>
@@ -3872,6 +4016,9 @@
       <c r="B93" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D93" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="E93" s="3" t="s">
         <v>52</v>
       </c>
@@ -3889,6 +4036,9 @@
       <c r="B94" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D94" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="E94" s="3" t="s">
         <v>68</v>
       </c>
@@ -3920,6 +4070,9 @@
       <c r="B96" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D96" s="18" t="s">
+        <v>76</v>
+      </c>
       <c r="E96" s="3" t="s">
         <v>48</v>
       </c>
@@ -3931,6 +4084,9 @@
       <c r="B97" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D97" s="18" t="s">
+        <v>76</v>
+      </c>
       <c r="E97" s="3" t="s">
         <v>47</v>
       </c>
@@ -3942,6 +4098,9 @@
       <c r="B98" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D98" s="18" t="s">
+        <v>76</v>
+      </c>
       <c r="E98" s="3" t="s">
         <v>51</v>
       </c>
@@ -3967,6 +4126,9 @@
       <c r="B100" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D100" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="E100" s="3" t="s">
         <v>48</v>
       </c>
@@ -3978,6 +4140,9 @@
       <c r="B101" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D101" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="E101" s="3" t="s">
         <v>47</v>
       </c>
@@ -3989,6 +4154,9 @@
       <c r="B102" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D102" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="E102" s="3" t="s">
         <v>51</v>
       </c>
@@ -4000,6 +4168,9 @@
       <c r="B103" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D103" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="E103" s="3" t="s">
         <v>52</v>
       </c>
@@ -4017,6 +4188,9 @@
       <c r="B104" s="18" t="s">
         <v>72</v>
       </c>
+      <c r="D104" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="E104" s="3" t="s">
         <v>68</v>
       </c>
@@ -4072,24 +4246,30 @@
         <v>47</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B108" s="18" t="s">
         <v>78</v>
       </c>
+      <c r="D108" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="E108" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B109" s="18" t="s">
         <v>78</v>
       </c>
+      <c r="D109" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="E109" s="3" t="s">
         <v>47</v>
       </c>
@@ -4115,6 +4295,9 @@
       <c r="B111" s="18" t="s">
         <v>78</v>
       </c>
+      <c r="D111" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="E111" s="3" t="s">
         <v>48</v>
       </c>
@@ -4140,6 +4323,9 @@
       <c r="B113" s="18" t="s">
         <v>78</v>
       </c>
+      <c r="D113" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="E113" s="3" t="s">
         <v>48</v>
       </c>
@@ -4151,6 +4337,9 @@
       <c r="B114" s="18" t="s">
         <v>78</v>
       </c>
+      <c r="D114" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="E114" s="3" t="s">
         <v>51</v>
       </c>
@@ -4161,6 +4350,9 @@
       </c>
       <c r="B115" s="18" t="s">
         <v>78</v>
+      </c>
+      <c r="D115" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>52</v>

</xml_diff>